<commit_message>
Automatische test-sync: 2025-06-18 09:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -684,8 +684,40 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-06-18 08:30:11</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -705,7 +737,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -723,7 +755,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -753,6 +785,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-18 09:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -716,8 +716,40 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-06-18 09:00:12</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -737,7 +769,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -755,7 +787,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -795,6 +827,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-18 10:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -748,8 +748,40 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-06-18 09:30:12</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -769,7 +801,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -787,7 +819,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -837,6 +869,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-18 11:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -780,8 +780,72 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-06-18 10:30:11</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-06-18 10:30:12</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -801,7 +865,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -842,17 +906,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Klacht</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Afmelding</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -862,7 +926,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Afmelding</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -872,7 +936,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Klacht</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-18 11:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -844,8 +844,48 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Onze openingstijden zijn maandag tot en met vrijdag van 09:00 tot 18:00 uur. Voor meer informatie of vragen zijn wij bereikbaar via e-mail of telefoon.
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-06-18 11:00:13</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -865,7 +905,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -883,7 +923,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -943,6 +983,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-18 12:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -884,8 +884,40 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-06-18 11:30:12</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -905,7 +937,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -956,17 +988,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Afmelding</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Afmelding</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-18 12:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -916,8 +916,40 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-06-18 12:00:11</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -937,7 +969,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -988,7 +1020,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Afmelding</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -998,11 +1030,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Afmelding</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-18 13:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -948,8 +948,40 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-06-18 12:30:11</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -969,7 +1001,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1010,7 +1042,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Klacht</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1020,11 +1052,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Klacht</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-18 13:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -980,8 +980,40 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-06-18 13:00:11</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1001,7 +1033,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1046,7 +1078,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-18 14:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1012,8 +1012,72 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-06-18 14:00:12</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-06-18 14:00:13</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1033,7 +1097,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1078,7 +1142,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -1088,7 +1152,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-18 15:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1076,8 +1076,72 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-06-18 15:00:11</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-06-18 15:00:11</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1097,7 +1161,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1142,7 +1206,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-18 16:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1140,8 +1140,40 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-06-18 15:30:11</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1161,7 +1193,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1206,7 +1238,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-18 16:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1172,8 +1172,40 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-06-18 16:00:11</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1193,7 +1225,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1258,7 +1290,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 08:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-18.xlsx
+++ b/logs/mail_log_2025-06-18.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1204,8 +1204,40 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-06-18 16:30:10</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1225,7 +1257,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1270,7 +1302,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">

</xml_diff>